<commit_message>
Updated dataset from Justin
From Justin's email, 2/13/2015:

"Attached is the RIGHT data for 126C and 54C. I looked into it and I
don't know what I was thinking on December 3rd, but for the 126C, I sent
you the moving average of 5 points instead of the absolute calculations
for FRET at each time point. Apologies!
Attached is the proper data."
</commit_message>
<xml_diff>
--- a/tbidbaxlipo/data/2014-12-3 - Bax-Bax FRET with NBD and TbDPA RLS 126C and 54C.xlsx
+++ b/tbidbaxlipo/data/2014-12-3 - Bax-Bax FRET with NBD and TbDPA RLS 126C and 54C.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12075"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="14880" windowHeight="20060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,25 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+  <si>
+    <t>126C</t>
+  </si>
+  <si>
+    <t>54C</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
   <si>
     <t>RLS</t>
   </si>
@@ -27,32 +41,24 @@
     <t>NBD</t>
   </si>
   <si>
-    <t>Bax 126C</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>TB</t>
-  </si>
-  <si>
     <t>DAC</t>
-  </si>
-  <si>
-    <t>Bax 54C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,7 +91,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -373,48 +379,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H174"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:H128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -425,10 +434,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>9.4532684774195825</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1.7603661947806815</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -451,10 +460,10 @@
         <v>8.673143575113162</v>
       </c>
       <c r="C4">
-        <v>11.777264880959516</v>
+        <v>6.5132786519519259</v>
       </c>
       <c r="D4">
-        <v>1.9826774357780337</v>
+        <v>1.6024160797200757</v>
       </c>
       <c r="E4">
         <v>29.018000000000029</v>
@@ -477,10 +486,10 @@
         <v>14.24345989669149</v>
       </c>
       <c r="C5">
-        <v>13.692894081182386</v>
+        <v>6.3177301462430835</v>
       </c>
       <c r="D5">
-        <v>2.1279943331396249</v>
+        <v>1.7715711395971492</v>
       </c>
       <c r="E5">
         <v>58.190000000000055</v>
@@ -503,10 +512,10 @@
         <v>21.039010902963952</v>
       </c>
       <c r="C6">
-        <v>15.727262966911658</v>
+        <v>10.037134755078526</v>
       </c>
       <c r="D6">
-        <v>2.2581296102822108</v>
+        <v>1.9107581630316364</v>
       </c>
       <c r="E6">
         <v>86.995000000000005</v>
@@ -529,10 +538,10 @@
         <v>27.50742794172638</v>
       </c>
       <c r="C7">
-        <v>17.206333394259179</v>
+        <v>13.957034394680679</v>
       </c>
       <c r="D7">
-        <v>2.384504089336192</v>
+        <v>2.0671207980043342</v>
       </c>
       <c r="E7">
         <v>115.93500000000006</v>
@@ -555,10 +564,10 @@
         <v>31.569239195234864</v>
       </c>
       <c r="C8">
-        <v>18.335660462534495</v>
+        <v>11.321493945916783</v>
       </c>
       <c r="D8">
-        <v>2.4926384657673015</v>
+        <v>2.2103309883308917</v>
       </c>
       <c r="E8">
         <v>144.75300000000004</v>
@@ -581,10 +590,10 @@
         <v>34.79164155469622</v>
       </c>
       <c r="C9">
-        <v>20.198068547172685</v>
+        <v>14.164013744442649</v>
       </c>
       <c r="D9">
-        <v>2.5928634201702412</v>
+        <v>2.3338674459841156</v>
       </c>
       <c r="E9">
         <v>173.83500000000004</v>
@@ -607,10 +616,10 @@
         <v>37.677590860172053</v>
       </c>
       <c r="C10">
-        <v>21.970626456742917</v>
+        <v>18.188425085002812</v>
       </c>
       <c r="D10">
-        <v>2.6867294245344522</v>
+        <v>2.4743174638896219</v>
       </c>
       <c r="E10">
         <v>202.81900000000007</v>
@@ -633,10 +642,10 @@
         <v>39.519158619498029</v>
       </c>
       <c r="C11">
-        <v>23.443755089050274</v>
+        <v>18.716556932224691</v>
       </c>
       <c r="D11">
-        <v>2.7736406398971543</v>
+        <v>2.5523828024526649</v>
       </c>
       <c r="E11">
         <v>231.79100000000005</v>
@@ -659,10 +668,10 @@
         <v>41.895007711126887</v>
       </c>
       <c r="C12">
-        <v>24.735644901260958</v>
+        <v>19.05159528954341</v>
       </c>
       <c r="D12">
-        <v>2.8637874800954317</v>
+        <v>2.6690050373555243</v>
       </c>
       <c r="E12">
         <v>260.74099999999999</v>
@@ -685,10 +694,10 @@
         <v>43.844552407751578</v>
       </c>
       <c r="C13">
-        <v>25.822021435211795</v>
+        <v>20.83992117224096</v>
       </c>
       <c r="D13">
-        <v>2.9413682251999895</v>
+        <v>2.7159270565909925</v>
       </c>
       <c r="E13">
         <v>289.72300000000007</v>
@@ -711,10 +720,10 @@
         <v>45.416280847554866</v>
       </c>
       <c r="C14">
-        <v>26.41407932607126</v>
+        <v>22.672274725265428</v>
       </c>
       <c r="D14">
-        <v>3.0184676528445338</v>
+        <v>2.8116807147485279</v>
       </c>
       <c r="E14">
         <v>318.80000000000007</v>
@@ -737,10 +746,10 @@
         <v>46.407019779734426</v>
       </c>
       <c r="C15">
-        <v>26.997191404747838</v>
+        <v>24.967186484181269</v>
       </c>
       <c r="D15">
-        <v>3.0926596882782871</v>
+        <v>2.8970634721693806</v>
       </c>
       <c r="E15">
         <v>347.73900000000003</v>
@@ -763,10 +772,10 @@
         <v>46.332438976957832</v>
       </c>
       <c r="C16">
-        <v>26.904946897507703</v>
+        <v>27.166672281750216</v>
       </c>
       <c r="D16">
-        <v>3.167852625514513</v>
+        <v>2.9957847560658362</v>
       </c>
       <c r="E16">
         <v>376.76900000000001</v>
@@ -789,10 +798,10 @@
         <v>49.33917275828852</v>
       </c>
       <c r="C17">
-        <v>27.656989923328791</v>
+        <v>26.590211568086154</v>
       </c>
       <c r="D17">
-        <v>3.2344972239599792</v>
+        <v>3.0932638436423265</v>
       </c>
       <c r="E17">
         <v>405.73200000000008</v>
@@ -815,10 +824,10 @@
         <v>49.711596493213825</v>
       </c>
       <c r="C18">
-        <v>27.453873548960548</v>
+        <v>25.672712316695943</v>
       </c>
       <c r="D18">
-        <v>3.2919516459917233</v>
+        <v>3.1344895079828765</v>
       </c>
       <c r="E18">
         <v>434.86300000000006</v>
@@ -841,10 +850,10 @@
         <v>49.548752918424363</v>
       </c>
       <c r="C19">
-        <v>27.429910228997084</v>
+        <v>24.448324391310383</v>
       </c>
       <c r="D19">
-        <v>3.3606533367236984</v>
+        <v>3.1785236224582563</v>
       </c>
       <c r="E19">
         <v>463.779</v>
@@ -867,10 +876,10 @@
         <v>50.674289646308445</v>
       </c>
       <c r="C20">
-        <v>29.893788141917579</v>
+        <v>26.226156084266261</v>
       </c>
       <c r="D20">
-        <v>3.4220389569187772</v>
+        <v>3.2568329273510472</v>
       </c>
       <c r="E20">
         <v>492.74400000000003</v>
@@ -893,10 +902,10 @@
         <v>51.386652494876692</v>
       </c>
       <c r="C21">
-        <v>30.299678000607049</v>
+        <v>24.404985756844333</v>
       </c>
       <c r="D21">
-        <v>3.4879017579674425</v>
+        <v>3.348221095586736</v>
       </c>
       <c r="E21">
         <v>521.73900000000003</v>
@@ -919,10 +928,10 @@
         <v>51.923340305867342</v>
       </c>
       <c r="C22">
-        <v>31.115818871944043</v>
+        <v>31.750133657988577</v>
       </c>
       <c r="D22">
-        <v>3.5390470614034153</v>
+        <v>3.3956523467386308</v>
       </c>
       <c r="E22">
         <v>550.71</v>
@@ -945,10 +954,10 @@
         <v>53.072568004503907</v>
       </c>
       <c r="C23">
-        <v>30.242512139313131</v>
+        <v>25.352282320910479</v>
       </c>
       <c r="D23">
-        <v>3.5893823189155918</v>
+        <v>3.437990375832793</v>
       </c>
       <c r="E23">
         <v>579.59500000000003</v>
@@ -971,10 +980,10 @@
         <v>53.053306904361833</v>
       </c>
       <c r="C24">
-        <v>30.091522544061359</v>
+        <v>25.526663556548112</v>
       </c>
       <c r="D24">
-        <v>3.6370034034193104</v>
+        <v>3.5466996523747283</v>
       </c>
       <c r="E24">
         <v>608.64699999999993</v>
@@ -997,10 +1006,10 @@
         <v>53.366723913446258</v>
       </c>
       <c r="C25">
-        <v>31.898839203216028</v>
+        <v>39.46487113384277</v>
       </c>
       <c r="D25">
-        <v>3.6780775321393402</v>
+        <v>3.5468373436287268</v>
       </c>
       <c r="E25">
         <v>637.702</v>
@@ -1023,10 +1032,10 @@
         <v>54.384181128886851</v>
       </c>
       <c r="C26">
-        <v>30.53428917479388</v>
+        <v>28.69992477360266</v>
       </c>
       <c r="D26">
-        <v>3.726849956298075</v>
+        <v>3.652009733643041</v>
       </c>
       <c r="E26">
         <v>666.52</v>
@@ -1049,10 +1058,10 @@
         <v>53.80614476865243</v>
       </c>
       <c r="C27">
-        <v>31.553593544196719</v>
+        <v>29.37910297209071</v>
       </c>
       <c r="D27">
-        <v>3.7658548984735805</v>
+        <v>3.6550929162025705</v>
       </c>
       <c r="E27">
         <v>695.4380000000001</v>
@@ -1075,10 +1084,10 @@
         <v>54.269335544576734</v>
       </c>
       <c r="C28">
-        <v>32.446544101572691</v>
+        <v>26.427608827374726</v>
       </c>
       <c r="D28">
-        <v>3.806741466123682</v>
+        <v>3.6976638918116933</v>
       </c>
       <c r="E28">
         <v>724.34500000000003</v>
@@ -1101,10 +1110,10 @@
         <v>55.089503075973198</v>
       </c>
       <c r="C29">
-        <v>33.728489364038559</v>
+        <v>24.432049097160057</v>
       </c>
       <c r="D29">
-        <v>3.8458157384790135</v>
+        <v>3.7237168828551028</v>
       </c>
       <c r="E29">
         <v>753.26300000000015</v>
@@ -1127,10 +1136,10 @@
         <v>55.727203480323119</v>
       </c>
       <c r="C30">
-        <v>35.372523606397479</v>
+        <v>36.541679742388332</v>
       </c>
       <c r="D30">
-        <v>3.8920452760444419</v>
+        <v>3.793144424694904</v>
       </c>
       <c r="E30">
         <v>782.10500000000002</v>
@@ -1153,10 +1162,10 @@
         <v>55.710149091531477</v>
       </c>
       <c r="C31">
-        <v>35.108572348493446</v>
+        <v>31.148375751960511</v>
       </c>
       <c r="D31">
-        <v>3.9261351325291494</v>
+        <v>3.8394718885811407</v>
       </c>
       <c r="E31">
         <v>810.97299999999996</v>
@@ -1179,10 +1188,10 @@
         <v>56.430343238396816</v>
       </c>
       <c r="C32">
-        <v>35.518254911451699</v>
+        <v>34.912258439868694</v>
       </c>
       <c r="D32">
-        <v>3.9594560247428929</v>
+        <v>3.8860393866960683</v>
       </c>
       <c r="E32">
         <v>839.87599999999998</v>
@@ -1205,10 +1214,10 @@
         <v>57.159798754527927</v>
       </c>
       <c r="C33">
-        <v>35.788042136912253</v>
+        <v>34.821350622954427</v>
       </c>
       <c r="D33">
-        <v>3.9772261494953067</v>
+        <v>3.9004123221031821</v>
       </c>
       <c r="E33">
         <v>868.74400000000014</v>
@@ -1231,10 +1240,10 @@
         <v>56.842835277100235</v>
       </c>
       <c r="C34">
-        <v>36.100546705196116</v>
+        <v>34.240654617605728</v>
       </c>
       <c r="D34">
-        <v>4.0017117851938186</v>
+        <v>3.9321095259436847</v>
       </c>
       <c r="E34">
         <v>897.86900000000014</v>
@@ -1257,10 +1266,10 @@
         <v>56.814018838691517</v>
       </c>
       <c r="C35">
-        <v>36.233360749447321</v>
+        <v>34.451911249113657</v>
       </c>
       <c r="D35">
-        <v>4.0362838469837845</v>
+        <v>4.0010941082476723</v>
       </c>
       <c r="E35">
         <v>926.78600000000006</v>
@@ -1283,10 +1292,10 @@
         <v>57.131295125452809</v>
       </c>
       <c r="C36">
-        <v>35.863047690106214</v>
+        <v>34.932981364404228</v>
       </c>
       <c r="D36">
-        <v>4.0669301430194551</v>
+        <v>3.9976835636031458</v>
       </c>
       <c r="E36">
         <v>955.67399999999998</v>
@@ -1309,10 +1318,10 @@
         <v>57.891992399013105</v>
       </c>
       <c r="C37">
-        <v>35.979634506767944</v>
+        <v>33.645259759078719</v>
       </c>
       <c r="D37">
-        <v>4.0980833761173168</v>
+        <v>4.0393972418636039</v>
       </c>
       <c r="E37">
         <v>984.80099999999993</v>
@@ -1335,10 +1344,10 @@
         <v>58.310577640557746</v>
       </c>
       <c r="C38">
-        <v>35.881419655545535</v>
+        <v>36.556525170952192</v>
       </c>
       <c r="D38">
-        <v>4.1289117782415401</v>
+        <v>3.9926601352105542</v>
       </c>
       <c r="E38">
         <v>1013.768</v>
@@ -1361,10 +1370,10 @@
         <v>58.526021929013275</v>
       </c>
       <c r="C39">
-        <v>36.417170812280858</v>
+        <v>36.725965876933131</v>
       </c>
       <c r="D39">
-        <v>4.160694689244572</v>
+        <v>4.0473261362942523</v>
       </c>
       <c r="E39">
         <v>1042.7329999999999</v>
@@ -1387,10 +1396,10 @@
         <v>57.810238812425617</v>
       </c>
       <c r="C40">
-        <v>36.82051552935387</v>
+        <v>35.050113679316667</v>
       </c>
       <c r="D40">
-        <v>4.1847657915033141</v>
+        <v>4.1395418966834807</v>
       </c>
       <c r="E40">
         <v>1071.7740000000001</v>
@@ -1413,10 +1422,10 @@
         <v>58.546135928026665</v>
       </c>
       <c r="C41">
-        <v>38.078597655330348</v>
+        <v>32.194971757183012</v>
       </c>
       <c r="D41">
-        <v>4.2043322980531102</v>
+        <v>4.1849718844616888</v>
       </c>
       <c r="E41">
         <v>1100.799</v>
@@ -1439,10 +1448,10 @@
         <v>58.496616356391193</v>
       </c>
       <c r="C42">
-        <v>39.204379641278699</v>
+        <v>35.643540671252651</v>
       </c>
       <c r="D42">
-        <v>4.2103984329681916</v>
+        <v>4.1846029621903202</v>
       </c>
       <c r="E42">
         <v>1129.8500000000001</v>
@@ -1465,10 +1474,10 @@
         <v>58.438422755385908</v>
       </c>
       <c r="C43">
-        <v>39.858229151793445</v>
+        <v>33.046671697365845</v>
       </c>
       <c r="D43">
-        <v>4.2226469804289186</v>
+        <v>4.2243676546089386</v>
       </c>
       <c r="E43">
         <v>1158.7329999999999</v>
@@ -1491,10 +1500,10 @@
         <v>58.983731663383018</v>
       </c>
       <c r="C44">
-        <v>40.610551714848</v>
+        <v>39.821756879590588</v>
       </c>
       <c r="D44">
-        <v>4.2347592135481866</v>
+        <v>4.1833576012287477</v>
       </c>
       <c r="E44">
         <v>1187.749</v>
@@ -1517,10 +1526,10 @@
         <v>59.4181012160522</v>
       </c>
       <c r="C45">
-        <v>41.473481644680476</v>
+        <v>39.184222743281282</v>
       </c>
       <c r="D45">
-        <v>4.2648455501027058</v>
+        <v>4.1917527498467058</v>
       </c>
       <c r="E45">
         <v>1216.691</v>
@@ -1543,10 +1552,10 @@
         <v>58.762474384653743</v>
       </c>
       <c r="C46">
-        <v>41.807247001634728</v>
+        <v>42.71772129558736</v>
       </c>
       <c r="D46">
-        <v>4.2909707350030617</v>
+        <v>4.2569409359822581</v>
       </c>
       <c r="E46">
         <v>1245.7850000000001</v>
@@ -1569,10 +1578,10 @@
         <v>59.690290792317434</v>
       </c>
       <c r="C47">
-        <v>41.184542202716244</v>
+        <v>39.056252393387922</v>
       </c>
       <c r="D47">
-        <v>4.3122324691852798</v>
+        <v>4.2213686939521828</v>
       </c>
       <c r="E47">
         <v>1274.7360000000001</v>
@@ -1595,10 +1604,10 @@
         <v>60.002628220432207</v>
       </c>
       <c r="C48">
-        <v>40.908433123486986</v>
+        <v>39.628544021353044</v>
       </c>
       <c r="D48">
-        <v>4.3550922879391978</v>
+        <v>4.2580942469546814</v>
       </c>
       <c r="E48">
         <v>1303.6949999999999</v>
@@ -1621,10 +1630,10 @@
         <v>60.546128755541908</v>
       </c>
       <c r="C49">
-        <v>40.503769417349353</v>
+        <v>37.631836763511338</v>
       </c>
       <c r="D49">
-        <v>4.3777315215421551</v>
+        <v>4.2970410533245493</v>
       </c>
       <c r="E49">
         <v>1332.7750000000001</v>
@@ -1647,10 +1656,10 @@
         <v>59.493574691735851</v>
       </c>
       <c r="C50">
-        <v>40.902010154153174</v>
+        <v>45.081038420655204</v>
       </c>
       <c r="D50">
-        <v>4.4018215544672925</v>
+        <v>4.3638756205558602</v>
       </c>
       <c r="E50">
         <v>1361.7280000000001</v>
@@ -1673,10 +1682,10 @@
         <v>60.603929999142146</v>
       </c>
       <c r="C51">
-        <v>40.313426109519092</v>
+        <v>41.21841569474973</v>
       </c>
       <c r="D51">
-        <v>4.4137873608382518</v>
+        <v>4.3485038592488401</v>
       </c>
       <c r="E51">
         <v>1390.7540000000001</v>
@@ -1699,10 +1708,10 @@
         <v>60.30346048537114</v>
       </c>
       <c r="C52">
-        <v>40.327787609730684</v>
+        <v>38.922534987563317</v>
       </c>
       <c r="D52">
-        <v>4.4321480757327478</v>
+        <v>4.3845113410755703</v>
       </c>
       <c r="E52">
         <v>1419.7360000000001</v>
@@ -1725,10 +1734,10 @@
         <v>59.263733996665536</v>
       </c>
       <c r="C53">
-        <v>40.470282089935587</v>
+        <v>37.373455988362615</v>
       </c>
       <c r="D53">
-        <v>4.4413057404574792</v>
+        <v>4.4785276064756872</v>
       </c>
       <c r="E53">
         <v>1448.722</v>
@@ -1751,10 +1760,10 @@
         <v>60.449684195232933</v>
       </c>
       <c r="C54">
-        <v>41.446713866856051</v>
+        <v>37.162248339104984</v>
       </c>
       <c r="D54">
-        <v>4.4403127306963359</v>
+        <v>4.3939296485724189</v>
       </c>
       <c r="E54">
         <v>1477.837</v>
@@ -1777,10 +1786,10 @@
         <v>61.122800836445698</v>
       </c>
       <c r="C55">
-        <v>42.341019765906573</v>
+        <v>40.058986504833861</v>
       </c>
       <c r="D55">
-        <v>4.4530345372928677</v>
+        <v>4.4415812508753838</v>
       </c>
       <c r="E55">
         <v>1506.7619999999999</v>
@@ -1803,10 +1812,10 @@
         <v>60.801421842946809</v>
       </c>
       <c r="C56">
-        <v>42.644245984662021</v>
+        <v>41.493807181717699</v>
       </c>
       <c r="D56">
-        <v>4.4608935552931408</v>
+        <v>4.4356704587816154</v>
       </c>
       <c r="E56">
         <v>1535.7990000000002</v>
@@ -1829,10 +1838,10 @@
         <v>60.952233323350313</v>
       </c>
       <c r="C57">
-        <v>42.385820469280418</v>
+        <v>41.305944438803706</v>
       </c>
       <c r="D57">
-        <v>4.4621018825742658</v>
+        <v>4.4586681486158142</v>
       </c>
       <c r="E57">
         <v>1564.8419999999999</v>
@@ -1855,10 +1864,10 @@
         <v>60.985297210100327</v>
       </c>
       <c r="C58">
-        <v>42.577886165988843</v>
+        <v>39.790993205938854</v>
       </c>
       <c r="D58">
-        <v>4.4735107315848577</v>
+        <v>4.4394573294239557</v>
       </c>
       <c r="E58">
         <v>1593.8080000000002</v>
@@ -1881,10 +1890,10 @@
         <v>61.320535511205307</v>
       </c>
       <c r="C59">
-        <v>43.440474867181592</v>
+        <v>43.32449493478515</v>
       </c>
       <c r="D59">
-        <v>4.4935960331977371</v>
+        <v>4.4725695479088259</v>
       </c>
       <c r="E59">
         <v>1622.5670000000002</v>
@@ -1907,10 +1916,10 @@
         <v>62.132212033606883</v>
       </c>
       <c r="C60">
-        <v>44.777559725365563</v>
+        <v>42.612756363383056</v>
       </c>
       <c r="D60">
-        <v>4.4992464684356532</v>
+        <v>4.4702604881516113</v>
       </c>
       <c r="E60">
         <v>1651.6119999999999</v>
@@ -1933,10 +1942,10 @@
         <v>61.274191881369774</v>
       </c>
       <c r="C61">
-        <v>44.474725444212062</v>
+        <v>41.907053190128806</v>
       </c>
       <c r="D61">
-        <v>4.5226694963347986</v>
+        <v>4.488735358877018</v>
       </c>
       <c r="E61">
         <v>1680.722</v>
@@ -1959,10 +1968,10 @@
         <v>61.523494341078198</v>
       </c>
       <c r="C62">
-        <v>44.125646296833644</v>
+        <v>39.918786434609707</v>
       </c>
       <c r="D62">
-        <v>4.5577122063936217</v>
+        <v>4.4429204224683687</v>
       </c>
       <c r="E62">
         <v>1709.691</v>
@@ -1985,10 +1994,10 @@
         <v>61.864793248258266</v>
       </c>
       <c r="C63">
-        <v>44.551098050848729</v>
+        <v>42.476523344980322</v>
       </c>
       <c r="D63">
-        <v>4.5832426252696035</v>
+        <v>4.5271212426793683</v>
       </c>
       <c r="E63">
         <v>1738.8280000000002</v>
@@ -2011,10 +2020,10 @@
         <v>61.727046790957949</v>
       </c>
       <c r="C64">
-        <v>44.022569140408876</v>
+        <v>45.0481950677339</v>
       </c>
       <c r="D64">
-        <v>4.6028966673412031</v>
+        <v>4.5599691391012351</v>
       </c>
       <c r="E64">
         <v>1767.8340000000001</v>
@@ -2037,10 +2046,10 @@
         <v>61.711295076599527</v>
       </c>
       <c r="C65">
-        <v>43.434554965864635</v>
+        <v>51.473598900676208</v>
       </c>
       <c r="D65">
-        <v>4.6177308308286511</v>
+        <v>4.5064721593363188</v>
       </c>
       <c r="E65">
         <v>1796.7839999999999</v>
@@ -2063,10 +2072,10 @@
         <v>61.062238138365174</v>
       </c>
       <c r="C66">
-        <v>42.939908850232911</v>
+        <v>40.767078412241197</v>
       </c>
       <c r="D66">
-        <v>4.6385308252909043</v>
+        <v>4.6107986555464802</v>
       </c>
       <c r="E66">
         <v>1825.6940000000002</v>
@@ -2089,10 +2098,10 @@
         <v>59.872133795961325</v>
       </c>
       <c r="C67">
-        <v>43.146021912845718</v>
+        <v>39.779527590762562</v>
       </c>
       <c r="D67">
-        <v>4.6489226250017452</v>
+        <v>4.698991619229961</v>
       </c>
       <c r="E67">
         <v>1854.7450000000001</v>
@@ -2115,10 +2124,10 @@
         <v>60.959340614576064</v>
       </c>
       <c r="C68">
-        <v>43.517013480899038</v>
+        <v>42.511778610625107</v>
       </c>
       <c r="D68">
-        <v>4.6419962056654391</v>
+        <v>4.5961029357242564</v>
       </c>
       <c r="E68">
         <v>1883.7239999999999</v>
@@ -2141,10 +2150,10 @@
         <v>61.011871050810576</v>
       </c>
       <c r="C69">
-        <v>45.692756853285829</v>
+        <v>39.255308914354494</v>
       </c>
       <c r="D69">
-        <v>4.6555306841009374</v>
+        <v>4.6450454951089704</v>
       </c>
       <c r="E69">
         <v>1912.847</v>
@@ -2167,10 +2176,10 @@
         <v>61.811982300403379</v>
       </c>
       <c r="C70">
-        <v>46.981815587501181</v>
+        <v>41.46443700447464</v>
       </c>
       <c r="D70">
-        <v>4.6522414657662869</v>
+        <v>4.648974120025918</v>
       </c>
       <c r="E70">
         <v>1941.704</v>
@@ -2193,10 +2202,10 @@
         <v>61.717163989765609</v>
       </c>
       <c r="C71">
-        <v>47.489931588926531</v>
+        <v>48.458889252343226</v>
       </c>
       <c r="D71">
-        <v>4.6543446281920433</v>
+        <v>4.63127212610984</v>
       </c>
       <c r="E71">
         <v>1970.787</v>
@@ -2219,10 +2228,10 @@
         <v>62.858583417178401</v>
       </c>
       <c r="C72">
-        <v>47.22186903155373</v>
+        <v>42.023271514480989</v>
       </c>
       <c r="D72">
-        <v>4.6617324787597134</v>
+        <v>4.6731494538115257</v>
       </c>
       <c r="E72">
         <v>1999.7259999999999</v>
@@ -2245,10 +2254,10 @@
         <v>61.863246546658537</v>
       </c>
       <c r="C73">
-        <v>47.037013273392596</v>
+        <v>42.040602375979752</v>
       </c>
       <c r="D73">
-        <v>4.6572873160133534</v>
+        <v>4.6574331032121226</v>
       </c>
       <c r="E73">
         <v>2028.7340000000002</v>
@@ -2271,10 +2280,10 @@
         <v>62.78975908367741</v>
       </c>
       <c r="C74">
-        <v>47.74443129413924</v>
+        <v>55.772237613025212</v>
       </c>
       <c r="D74">
-        <v>4.6616787490742055</v>
+        <v>4.6773098063372514</v>
       </c>
       <c r="E74">
         <v>2057.8130000000001</v>
@@ -2297,10 +2306,10 @@
         <v>62.008698400984962</v>
       </c>
       <c r="C75">
-        <v>46.554895370564793</v>
+        <v>47.111709036578873</v>
       </c>
       <c r="D75">
-        <v>4.6596987337934861</v>
+        <v>4.6253101851010623</v>
       </c>
       <c r="E75">
         <v>2086.92</v>
@@ -2323,10 +2332,10 @@
         <v>62.304190777338228</v>
       </c>
       <c r="C76">
-        <v>46.411718026631206</v>
+        <v>44.561241292552403</v>
       </c>
       <c r="D76">
-        <v>4.6694285922058709</v>
+        <v>4.6615930945804616</v>
       </c>
       <c r="E76">
         <v>2115.8519999999999</v>
@@ -2349,10 +2358,10 @@
         <v>62.39495781833724</v>
       </c>
       <c r="C77">
-        <v>46.867265249380409</v>
+        <v>46.825133820873766</v>
       </c>
       <c r="D77">
-        <v>4.6778885159061057</v>
+        <v>4.6755992295158588</v>
       </c>
       <c r="E77">
         <v>2144.741</v>
@@ -2375,10 +2384,10 @@
         <v>62.926786019699897</v>
       </c>
       <c r="C78">
-        <v>46.507561470793782</v>
+        <v>40.896634874533746</v>
       </c>
       <c r="D78">
-        <v>4.6863027682450413</v>
+        <v>4.6464784773333676</v>
       </c>
       <c r="E78">
         <v>2173.6689999999999</v>
@@ -2401,10 +2410,10 @@
         <v>62.93511763349899</v>
       </c>
       <c r="C79">
-        <v>47.289247887984175</v>
+        <v>46.35208863889283</v>
       </c>
       <c r="D79">
-        <v>4.6979060026953627</v>
+        <v>4.6837817015772307</v>
       </c>
       <c r="E79">
         <v>2202.6660000000002</v>
@@ -2427,10 +2436,10 @@
         <v>62.528316870538973</v>
       </c>
       <c r="C80">
-        <v>47.083280128951792</v>
+        <v>48.522397146253091</v>
       </c>
       <c r="D80">
-        <v>4.7031764100722429</v>
+        <v>4.6654297146529347</v>
       </c>
       <c r="E80">
         <v>2231.6189999999997</v>
@@ -2453,10 +2462,10 @@
         <v>62.332594223691792</v>
       </c>
       <c r="C81">
-        <v>46.282292257147162</v>
+        <v>46.239088982486265</v>
       </c>
       <c r="D81">
-        <v>4.7106501483811369</v>
+        <v>4.6836893355753686</v>
       </c>
       <c r="E81">
         <v>2260.4390000000003</v>
@@ -2479,10 +2488,10 @@
         <v>62.291223843586295</v>
       </c>
       <c r="C82">
-        <v>47.041452954862073</v>
+        <v>47.337655711453444</v>
       </c>
       <c r="D82">
-        <v>4.7162134017305242</v>
+        <v>4.7123526367818718</v>
       </c>
       <c r="E82">
         <v>2289.37</v>
@@ -2505,10 +2514,10 @@
         <v>62.517205260979772</v>
       </c>
       <c r="C83">
-        <v>46.787635740608181</v>
+        <v>44.632854497175799</v>
       </c>
       <c r="D83">
-        <v>4.7283904776490795</v>
+        <v>4.7260847435494755</v>
       </c>
       <c r="E83">
         <v>2318.2030000000004</v>
@@ -2531,10 +2540,10 @@
         <v>62.77525232654245</v>
       </c>
       <c r="C84">
-        <v>47.375026111515631</v>
+        <v>45.660763226911605</v>
       </c>
       <c r="D84">
-        <v>4.7415550331062821</v>
+        <v>4.7160978840352978</v>
       </c>
       <c r="E84">
         <v>2347.0860000000002</v>
@@ -2557,10 +2566,10 @@
         <v>62.639751457469607</v>
       </c>
       <c r="C85">
-        <v>47.01288223617869</v>
+        <v>45.09678111543758</v>
       </c>
       <c r="D85">
-        <v>4.7486682009083934</v>
+        <v>4.7154041458385132</v>
       </c>
       <c r="E85">
         <v>2376.0100000000002</v>
@@ -2583,10 +2592,10 @@
         <v>62.49497725701498</v>
       </c>
       <c r="C86">
-        <v>47.104120540038878</v>
+        <v>43.640632609917596</v>
       </c>
       <c r="D86">
-        <v>4.7561821480730986</v>
+        <v>4.7102721445062938</v>
       </c>
       <c r="E86">
         <v>2404.8739999999998</v>
@@ -2609,10 +2618,10 @@
         <v>62.012712289011219</v>
       </c>
       <c r="C87">
-        <v>47.533756527539531</v>
+        <v>50.865930289252404</v>
       </c>
       <c r="D87">
-        <v>4.7638038330009751</v>
+        <v>4.7170688556716893</v>
       </c>
       <c r="E87">
         <v>2433.9089999999997</v>
@@ -2635,10 +2644,10 @@
         <v>61.734149297337297</v>
       </c>
       <c r="C88">
-        <v>46.90631157229609</v>
+        <v>45.790721083761184</v>
       </c>
       <c r="D88">
-        <v>4.7727668715143849</v>
+        <v>4.7854150922932064</v>
       </c>
       <c r="E88">
         <v>2462.8429999999998</v>
@@ -2661,10 +2670,10 @@
         <v>62.651480013161873</v>
       </c>
       <c r="C89">
-        <v>46.684985611253587</v>
+        <v>48.212810677062102</v>
       </c>
       <c r="D89">
-        <v>4.776413003637269</v>
+        <v>4.8050720762926922</v>
       </c>
       <c r="E89">
         <v>2491.8059999999996</v>
@@ -2687,10 +2696,10 @@
         <v>62.62431763634406</v>
       </c>
       <c r="C90">
-        <v>46.573789168708579</v>
+        <v>43.453612295040621</v>
       </c>
       <c r="D90">
-        <v>4.773005814746802</v>
+        <v>4.7587768908479671</v>
       </c>
       <c r="E90">
         <v>2520.723</v>
@@ -2713,10 +2722,10 @@
         <v>62.354207374893811</v>
       </c>
       <c r="C91">
-        <v>48.135638566717539</v>
+        <v>45.652849355442939</v>
       </c>
       <c r="D91">
-        <v>4.7732139015949206</v>
+        <v>4.760487828826748</v>
       </c>
       <c r="E91">
         <v>2549.7520000000004</v>
@@ -2739,10 +2748,10 @@
         <v>62.382299507178288</v>
       </c>
       <c r="C92">
-        <v>48.214126000388973</v>
+        <v>46.25912634889113</v>
       </c>
       <c r="D92">
-        <v>4.7724278049203859</v>
+        <v>4.7560022540735458</v>
       </c>
       <c r="E92">
         <v>2578.7139999999999</v>
@@ -2765,10 +2774,10 @@
         <v>62.421199710328267</v>
       </c>
       <c r="C93">
-        <v>48.067267917585973</v>
+        <v>47.041854246616452</v>
       </c>
       <c r="D93">
-        <v>4.7632265229169981</v>
+        <v>4.7708470867521493</v>
       </c>
       <c r="E93">
         <v>2607.7920000000004</v>
@@ -2791,10 +2800,10 @@
         <v>62.825865235581006</v>
       </c>
       <c r="C94">
-        <v>48.051628498257223</v>
+        <v>44.441810238015954</v>
       </c>
       <c r="D94">
-        <v>4.7562362163436589</v>
+        <v>4.8072918850305122</v>
       </c>
       <c r="E94">
         <v>2636.7390000000005</v>
@@ -2817,10 +2826,10 @@
         <v>62.892839926894339</v>
       </c>
       <c r="C95">
-        <v>48.07757304204241</v>
+        <v>47.535103974013182</v>
       </c>
       <c r="D95">
-        <v>4.7383633347903773</v>
+        <v>4.7846289429498867</v>
       </c>
       <c r="E95">
         <v>2665.7920000000004</v>
@@ -2843,10 +2852,10 @@
         <v>62.709819551982434</v>
       </c>
       <c r="C96">
-        <v>47.885592450570662</v>
+        <v>52.97258414303991</v>
       </c>
       <c r="D96">
-        <v>4.7325132171377158</v>
+        <v>4.7600254119366809</v>
       </c>
       <c r="E96">
         <v>2694.7200000000003</v>
@@ -2869,10 +2878,10 @@
         <v>62.994371975141227</v>
       </c>
       <c r="C97">
-        <v>46.802725425220785</v>
+        <v>46.131205125527153</v>
       </c>
       <c r="D97">
-        <v>4.7324284580133282</v>
+        <v>4.755771248779542</v>
       </c>
       <c r="E97">
         <v>2723.866</v>
@@ -2895,10 +2904,10 @@
         <v>63.376360917078877</v>
       </c>
       <c r="C98">
-        <v>47.180730555346997</v>
+        <v>45.364073370265302</v>
       </c>
       <c r="D98">
-        <v>4.7438599922223252</v>
+        <v>4.7007945620532166</v>
       </c>
       <c r="E98">
         <v>2752.8</v>
@@ -2921,10 +2930,10 @@
         <v>63.094354032206454</v>
       </c>
       <c r="C99">
-        <v>47.349143328168246</v>
+        <v>46.946536994838354</v>
       </c>
       <c r="D99">
-        <v>4.755096080091767</v>
+        <v>4.728905247312114</v>
       </c>
       <c r="E99">
         <v>2781.7529999999997</v>
@@ -2947,10 +2956,10 @@
         <v>62.599622146899868</v>
       </c>
       <c r="C100">
-        <v>47.225633286711854</v>
+        <v>44.599933922806045</v>
       </c>
       <c r="D100">
-        <v>4.7656243671986482</v>
+        <v>4.7000545957108271</v>
       </c>
       <c r="E100">
         <v>2810.8819999999996</v>
@@ -2973,10 +2982,10 @@
         <v>63.456268749166433</v>
       </c>
       <c r="C101">
-        <v>48.211981181730238</v>
+        <v>46.365043756996485</v>
       </c>
       <c r="D101">
-        <v>4.7791265671926366</v>
+        <v>4.749528237033914</v>
       </c>
       <c r="E101">
         <v>2839.799</v>
@@ -2999,10 +3008,10 @@
         <v>63.46058617588637</v>
       </c>
       <c r="C102">
-        <v>48.328065413011167</v>
+        <v>46.372856446776382</v>
       </c>
       <c r="D102">
-        <v>4.7813231414718578</v>
+        <v>4.7595168571903566</v>
       </c>
       <c r="E102">
         <v>2868.8029999999999</v>
@@ -3025,10 +3034,10 @@
         <v>63.299233080751428</v>
       </c>
       <c r="C103">
-        <v>48.589860416232192</v>
+        <v>48.435025325258117</v>
       </c>
       <c r="D103">
-        <v>4.783011070715407</v>
+        <v>4.8243604540335241</v>
       </c>
       <c r="E103">
         <v>2897.8059999999996</v>
@@ -3051,10 +3060,10 @@
         <v>63.353843130853818</v>
       </c>
       <c r="C104">
-        <v>47.542447086823934</v>
+        <v>46.39049528096465</v>
       </c>
       <c r="D104">
-        <v>4.7770289349893762</v>
+        <v>4.7682110892698679</v>
       </c>
       <c r="E104">
         <v>2926.8680000000004</v>
@@ -3077,10 +3086,10 @@
         <v>63.769363977330265</v>
       </c>
       <c r="C105">
-        <v>48.884093616159163</v>
+        <v>46.193782850253484</v>
       </c>
       <c r="D105">
-        <v>4.8031052131601699</v>
+        <v>4.792074969953398</v>
       </c>
       <c r="E105">
         <v>2955.8310000000001</v>
@@ -3103,10 +3112,10 @@
         <v>63.589225575217434</v>
       </c>
       <c r="C106">
-        <v>48.426653984013761</v>
+        <v>50.611408433077322</v>
       </c>
       <c r="D106">
-        <v>4.8120172908613759</v>
+        <v>4.7810677956747574</v>
       </c>
       <c r="E106">
         <v>2984.6549999999997</v>
@@ -3129,10 +3138,10 @@
         <v>64.123711758756926</v>
       </c>
       <c r="C107">
-        <v>47.811132284738825</v>
+        <v>47.072539966918171</v>
       </c>
       <c r="D107">
-        <v>4.82001142686926</v>
+        <v>4.7627076827092401</v>
       </c>
       <c r="E107">
         <v>3013.6559999999999</v>
@@ -3155,10 +3164,10 @@
         <v>64.444376912983088</v>
       </c>
       <c r="C108">
-        <v>49.475770269813971</v>
+        <v>47.968413143077981</v>
       </c>
       <c r="D108">
-        <v>4.8262781245202211</v>
+        <v>4.7696444326516527</v>
       </c>
       <c r="E108">
         <v>3042.7280000000001</v>
@@ -3181,10 +3190,10 @@
         <v>63.889647838630218</v>
       </c>
       <c r="C109">
-        <v>49.45916646219839</v>
+        <v>42.051376550564136</v>
       </c>
       <c r="D109">
-        <v>4.8388746019791657</v>
+        <v>4.7884676396773385</v>
       </c>
       <c r="E109">
         <v>3071.8909999999996</v>
@@ -3207,10 +3216,10 @@
         <v>62.686670166032187</v>
       </c>
       <c r="C110">
-        <v>50.52095344719627</v>
+        <v>54.567401171499696</v>
       </c>
       <c r="D110">
-        <v>4.839121249902516</v>
+        <v>4.9246687582946285</v>
       </c>
       <c r="E110">
         <v>3100.8</v>
@@ -3233,10 +3242,10 @@
         <v>63.327923617889169</v>
       </c>
       <c r="C111">
-        <v>49.467360588673777</v>
+        <v>43.405834802188039</v>
       </c>
       <c r="D111">
-        <v>4.8175927107002545</v>
+        <v>4.8455474361606354</v>
       </c>
       <c r="E111">
         <v>3129.7799999999997</v>
@@ -3259,10 +3268,10 @@
         <v>63.415853544024124</v>
       </c>
       <c r="C112">
-        <v>50.311121269110949</v>
+        <v>46.860000816760405</v>
       </c>
       <c r="D112">
-        <v>4.8147631178100285</v>
+        <v>4.829032611722063</v>
       </c>
       <c r="E112">
         <v>3158.7669999999998</v>
@@ -3285,10 +3294,10 @@
         <v>63.963046485292395</v>
       </c>
       <c r="C113">
-        <v>50.654113489476515</v>
+        <v>57.217975331711123</v>
       </c>
       <c r="D113">
-        <v>4.8103687954900769</v>
+        <v>4.8003078686150058</v>
       </c>
       <c r="E113">
         <v>3187.7259999999997</v>
@@ -3311,10 +3320,10 @@
         <v>63.926655635027842</v>
       </c>
       <c r="C114">
-        <v>49.508981375802158</v>
+        <v>47.867218253568275</v>
       </c>
       <c r="D114">
-        <v>4.8044797706530211</v>
+        <v>4.8452232974053215</v>
       </c>
       <c r="E114">
         <v>3216.7060000000001</v>
@@ -3337,10 +3346,10 @@
         <v>63.394565762377518</v>
       </c>
       <c r="C115">
-        <v>49.665158720594413</v>
+        <v>48.522628152448036</v>
       </c>
       <c r="D115">
-        <v>4.7936252982322971</v>
+        <v>4.7899475272174419</v>
       </c>
       <c r="E115">
         <v>3245.7259999999997</v>
@@ -3363,10 +3372,10 @@
         <v>63.986177329962835</v>
       </c>
       <c r="C116">
-        <v>49.634386137670852</v>
+        <v>48.146090146048806</v>
       </c>
       <c r="D116">
-        <v>4.7892780091379592</v>
+        <v>4.7954975230810613</v>
       </c>
       <c r="E116">
         <v>3274.6229999999996</v>
@@ -3389,10 +3398,10 @@
         <v>64.430195226350619</v>
       </c>
       <c r="C117">
-        <v>50.222966252861021</v>
+        <v>48.548285907761382</v>
       </c>
       <c r="D117">
-        <v>4.7910818548546841</v>
+        <v>4.8285698788192821</v>
       </c>
       <c r="E117">
         <v>3303.5889999999999</v>
@@ -3415,10 +3424,10 @@
         <v>63.895507182103508</v>
       </c>
       <c r="C118">
-        <v>50.319439996214136</v>
+        <v>48.950428545518818</v>
       </c>
       <c r="D118">
-        <v>4.78576254074824</v>
+        <v>4.8026666778023532</v>
       </c>
       <c r="E118">
         <v>3332.5829999999996</v>
@@ -3441,10 +3450,10 @@
         <v>64.224236596835993</v>
       </c>
       <c r="C119">
-        <v>50.211509553002372</v>
+        <v>50.2387618645215</v>
       </c>
       <c r="D119">
-        <v>4.7803898581136774</v>
+        <v>4.7649737195926649</v>
       </c>
       <c r="E119">
         <v>3361.7200000000003</v>
@@ -3467,10 +3476,10 @@
         <v>64.313961737530747</v>
       </c>
       <c r="C120">
-        <v>50.812152010652035</v>
+        <v>48.819069149223083</v>
       </c>
       <c r="D120">
-        <v>4.7893316786305702</v>
+        <v>4.7800964628809774</v>
       </c>
       <c r="E120">
         <v>3390.7669999999998</v>
@@ -3493,10 +3502,10 @@
         <v>64.227320430342672</v>
       </c>
       <c r="C121">
-        <v>51.349261138144506</v>
+        <v>48.335079115445524</v>
       </c>
       <c r="D121">
-        <v>4.7932784291339052</v>
+        <v>4.763863792651418</v>
       </c>
       <c r="E121">
         <v>3419.8460000000005</v>
@@ -3519,10 +3528,10 @@
         <v>64.747709858273353</v>
       </c>
       <c r="C122">
-        <v>51.300711259501732</v>
+        <v>51.733297436284118</v>
       </c>
       <c r="D122">
-        <v>4.7989438524034034</v>
+        <v>4.806320597381406</v>
       </c>
       <c r="E122">
         <v>3448.8379999999997</v>
@@ -3545,10 +3554,10 @@
         <v>64.590193013741953</v>
       </c>
       <c r="C123">
-        <v>50.91027398978121</v>
+        <v>49.13626247465708</v>
       </c>
       <c r="D123">
-        <v>4.8025595419681633</v>
+        <v>4.7966539941806259</v>
       </c>
       <c r="E123">
         <v>3477.7920000000004</v>
@@ -3571,10 +3580,10 @@
         <v>64.243044033728495</v>
       </c>
       <c r="C124">
-        <v>51.236902965413528</v>
+        <v>48.292627062363913</v>
       </c>
       <c r="D124">
-        <v>4.8012799161994479</v>
+        <v>4.7704305819949733</v>
       </c>
       <c r="E124">
         <v>3506.8540000000003</v>
@@ -3597,10 +3606,10 @@
         <v>64.833397784815645</v>
       </c>
       <c r="C125">
-        <v>51.634076010876335</v>
+        <v>53.899485268691571</v>
       </c>
       <c r="D125">
-        <v>4.800879136836854</v>
+        <v>4.8186246426940178</v>
       </c>
       <c r="E125">
         <v>3535.7349999999997</v>
@@ -3623,10 +3632,10 @@
         <v>64.343867027549038</v>
       </c>
       <c r="C126">
-        <v>50.516338099201533</v>
+        <v>52.092577254692209</v>
       </c>
       <c r="D126">
-        <v>4.7951052835858592</v>
+        <v>4.8037769659009868</v>
       </c>
       <c r="E126">
         <v>3564.5569999999998</v>
@@ -3649,10 +3658,10 @@
         <v>64.292377594460064</v>
       </c>
       <c r="C127">
-        <v>50.238572315802998</v>
+        <v>48.039183154789157</v>
       </c>
       <c r="D127">
-        <v>4.7941031094560076</v>
+        <v>4.7978563322684087</v>
       </c>
       <c r="E127">
         <v>3593.4650000000001</v>
@@ -3675,10 +3684,10 @@
         <v>64.4092286275188</v>
       </c>
       <c r="C128">
-        <v>50.578194496114314</v>
+        <v>49.353707327521221</v>
       </c>
       <c r="D128">
-        <v>4.7976647157019841</v>
+        <v>4.8280147347699645</v>
       </c>
       <c r="E128">
         <v>3622.3530000000001</v>
@@ -3693,679 +3702,54 @@
         <v>1.124696143678146</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129">
-        <v>3650.9520000000002</v>
-      </c>
-      <c r="B129">
-        <v>64.173668545732482</v>
-      </c>
-      <c r="C129">
-        <v>50.642272864372224</v>
-      </c>
-      <c r="D129">
-        <v>4.790156238566877</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
-      <c r="A130">
-        <v>3679.973</v>
-      </c>
-      <c r="B130">
-        <v>64.838944318955342</v>
-      </c>
-      <c r="C130">
-        <v>51.932793875579868</v>
-      </c>
-      <c r="D130">
-        <v>4.7982662910479368</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
-      <c r="A131">
-        <v>3708.8180000000002</v>
-      </c>
-      <c r="B131">
-        <v>64.700239995215725</v>
-      </c>
-      <c r="C131">
-        <v>51.995444486419359</v>
-      </c>
-      <c r="D131">
-        <v>4.8053117418398843</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
-      <c r="A132">
-        <v>3737.9849999999997</v>
-      </c>
-      <c r="B132">
-        <v>65.075943742350233</v>
-      </c>
-      <c r="C132">
-        <v>52.114573787794562</v>
-      </c>
-      <c r="D132">
-        <v>4.8154956277571879</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="A133">
-        <v>3766.9989999999998</v>
-      </c>
-      <c r="B133">
-        <v>64.553199272830625</v>
-      </c>
-      <c r="C133">
-        <v>51.887872193715872</v>
-      </c>
-      <c r="D133">
-        <v>4.8145397720622869</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
-      <c r="A134">
-        <v>3796.1329999999998</v>
-      </c>
-      <c r="B134">
-        <v>64.521448228312423</v>
-      </c>
-      <c r="C134">
-        <v>51.188769858158402</v>
-      </c>
-      <c r="D134">
-        <v>4.8193044763313821</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135">
-        <v>3825.0770000000002</v>
-      </c>
-      <c r="B135">
-        <v>64.471815016574865</v>
-      </c>
-      <c r="C135">
-        <v>50.857080812407851</v>
-      </c>
-      <c r="D135">
-        <v>4.8242071953913017</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="A136">
-        <v>3853.9949999999999</v>
-      </c>
-      <c r="B136">
-        <v>64.469039207555383</v>
-      </c>
-      <c r="C136">
-        <v>49.594191063614943</v>
-      </c>
-      <c r="D136">
-        <v>4.8132451507378775</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137">
-        <v>3882.8810000000003</v>
-      </c>
-      <c r="B137">
-        <v>64.082391918591568</v>
-      </c>
-      <c r="C137">
-        <v>49.181920183381699</v>
-      </c>
-      <c r="D137">
-        <v>4.8168300140147879</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138">
-        <v>3911.9409999999998</v>
-      </c>
-      <c r="B138">
-        <v>64.537481351449927</v>
-      </c>
-      <c r="C138">
-        <v>49.916013755431287</v>
-      </c>
-      <c r="D138">
-        <v>4.8037710745211024</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139">
-        <v>3940.857</v>
-      </c>
-      <c r="B139">
-        <v>64.356819606761761</v>
-      </c>
-      <c r="C139">
-        <v>50.250735109469311</v>
-      </c>
-      <c r="D139">
-        <v>4.8146107319648257</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="A140">
-        <v>3969.76</v>
-      </c>
-      <c r="B140">
-        <v>64.220844140736318</v>
-      </c>
-      <c r="C140">
-        <v>51.078567213305256</v>
-      </c>
-      <c r="D140">
-        <v>4.8124673004903586</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="A141">
-        <v>3998.6540000000005</v>
-      </c>
-      <c r="B141">
-        <v>64.408918509661305</v>
-      </c>
-      <c r="C141">
-        <v>51.725157675468722</v>
-      </c>
-      <c r="D141">
-        <v>4.809090787405494</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="A142">
-        <v>4027.5640000000003</v>
-      </c>
-      <c r="B142">
-        <v>64.878395975653262</v>
-      </c>
-      <c r="C142">
-        <v>51.614879675897214</v>
-      </c>
-      <c r="D142">
-        <v>4.8136772003109414</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="A143">
-        <v>4056.4470000000001</v>
-      </c>
-      <c r="B143">
-        <v>64.458866923155654</v>
-      </c>
-      <c r="C143">
-        <v>52.528439683474403</v>
-      </c>
-      <c r="D143">
-        <v>4.8155276278065458</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="A144">
-        <v>4085.3339999999998</v>
-      </c>
-      <c r="B144">
-        <v>64.423101990611187</v>
-      </c>
-      <c r="C144">
-        <v>52.112888104938719</v>
-      </c>
-      <c r="D144">
-        <v>4.8306760734622722</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
-      <c r="A145">
-        <v>4114.3290000000006</v>
-      </c>
-      <c r="B145">
-        <v>64.510350674239533</v>
-      </c>
-      <c r="C145">
-        <v>52.918924106338864</v>
-      </c>
-      <c r="D145">
-        <v>4.8344545321471273</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
-      <c r="A146">
-        <v>4143.2750000000005</v>
-      </c>
-      <c r="B146">
-        <v>64.629032509153191</v>
-      </c>
-      <c r="C146">
-        <v>52.389000210990112</v>
-      </c>
-      <c r="D146">
-        <v>4.844324519625876</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
-      <c r="A147">
-        <v>4172.2280000000001</v>
-      </c>
-      <c r="B147">
-        <v>64.587109180235259</v>
-      </c>
-      <c r="C147">
-        <v>52.444809945673114</v>
-      </c>
-      <c r="D147">
-        <v>4.8612021718049023</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4">
-      <c r="A148">
-        <v>4201.2359999999999</v>
-      </c>
-      <c r="B148">
-        <v>64.198644247744156</v>
-      </c>
-      <c r="C148">
-        <v>52.223690266844805</v>
-      </c>
-      <c r="D148">
-        <v>4.8797076656671265</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="A149">
-        <v>4230.1840000000002</v>
-      </c>
-      <c r="B149">
-        <v>64.401830955926982</v>
-      </c>
-      <c r="C149">
-        <v>51.157959539874689</v>
-      </c>
-      <c r="D149">
-        <v>4.8792604851043455</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="A150">
-        <v>4259.0280000000002</v>
-      </c>
-      <c r="B150">
-        <v>63.831972496300949</v>
-      </c>
-      <c r="C150">
-        <v>51.094449767352216</v>
-      </c>
-      <c r="D150">
-        <v>4.8834244943486214</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
-      <c r="A151">
-        <v>4287.9890000000005</v>
-      </c>
-      <c r="B151">
-        <v>63.949168636406505</v>
-      </c>
-      <c r="C151">
-        <v>49.591772519889751</v>
-      </c>
-      <c r="D151">
-        <v>4.8884681174584648</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
-      <c r="A152">
-        <v>4317.0030000000006</v>
-      </c>
-      <c r="B152">
-        <v>64.494935394393792</v>
-      </c>
-      <c r="C152">
-        <v>51.111377316624839</v>
-      </c>
-      <c r="D152">
-        <v>4.8820446398807524</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
-      <c r="A153">
-        <v>4346.0030000000006</v>
-      </c>
-      <c r="B153">
-        <v>64.231639950432921</v>
-      </c>
-      <c r="C153">
-        <v>50.247226745131691</v>
-      </c>
-      <c r="D153">
-        <v>4.8829160900845405</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
-      <c r="A154">
-        <v>4374.9530000000004</v>
-      </c>
-      <c r="B154">
-        <v>63.540793060874122</v>
-      </c>
-      <c r="C154">
-        <v>50.647187224018801</v>
-      </c>
-      <c r="D154">
-        <v>4.8829083327248206</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="A155">
-        <v>4403.942</v>
-      </c>
-      <c r="B155">
-        <v>64.408918509661305</v>
-      </c>
-      <c r="C155">
-        <v>52.437479585680002</v>
-      </c>
-      <c r="D155">
-        <v>4.8864860104745427</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
-      <c r="A156">
-        <v>4433.1010000000006</v>
-      </c>
-      <c r="B156">
-        <v>63.824262613481331</v>
-      </c>
-      <c r="C156">
-        <v>52.983054714570443</v>
-      </c>
-      <c r="D156">
-        <v>4.8813504502372327</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="A157">
-        <v>4462.0480000000007</v>
-      </c>
-      <c r="B157">
-        <v>64.270486922166668</v>
-      </c>
-      <c r="C157">
-        <v>53.18546964008916</v>
-      </c>
-      <c r="D157">
-        <v>4.8749342033313843</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="A158">
-        <v>4491.098</v>
-      </c>
-      <c r="B158">
-        <v>63.995119011678312</v>
-      </c>
-      <c r="C158">
-        <v>52.143321272143005</v>
-      </c>
-      <c r="D158">
-        <v>4.8703312148066713</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="A159">
-        <v>4520.0430000000006</v>
-      </c>
-      <c r="B159">
-        <v>64.418480726144651</v>
-      </c>
-      <c r="C159">
-        <v>52.765770978908506</v>
-      </c>
-      <c r="D159">
-        <v>4.8677554403187608</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
-      <c r="A160">
-        <v>4549.0929999999998</v>
-      </c>
-      <c r="B160">
-        <v>63.784167095889323</v>
-      </c>
-      <c r="C160">
-        <v>52.124202156198862</v>
-      </c>
-      <c r="D160">
-        <v>4.8518170757394818</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4">
-      <c r="A161">
-        <v>4578.1379999999999</v>
-      </c>
-      <c r="B161">
-        <v>64.586800856695163</v>
-      </c>
-      <c r="C161">
-        <v>50.660867384534903</v>
-      </c>
-      <c r="D161">
-        <v>4.8415861641206765</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
-      <c r="A162">
-        <v>4607.0550000000003</v>
-      </c>
-      <c r="B162">
-        <v>64.562143047916393</v>
-      </c>
-      <c r="C162">
-        <v>50.372280999538837</v>
-      </c>
-      <c r="D162">
-        <v>4.8458657362048507</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
-      <c r="A163">
-        <v>4636.0660000000007</v>
-      </c>
-      <c r="B163">
-        <v>64.063273167629973</v>
-      </c>
-      <c r="C163">
-        <v>50.883855679547452</v>
-      </c>
-      <c r="D163">
-        <v>4.8329671129706711</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4">
-      <c r="A164">
-        <v>4664.9639999999999</v>
-      </c>
-      <c r="B164">
-        <v>64.334619713769598</v>
-      </c>
-      <c r="C164">
-        <v>51.104724349099108</v>
-      </c>
-      <c r="D164">
-        <v>4.8421659270652437</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4">
-      <c r="A165">
-        <v>4693.9340000000002</v>
-      </c>
-      <c r="B165">
-        <v>64.280663991412794</v>
-      </c>
-      <c r="C165">
-        <v>51.145833338494128</v>
-      </c>
-      <c r="D165">
-        <v>4.8352030609292456</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4">
-      <c r="A166">
-        <v>4722.9140000000007</v>
-      </c>
-      <c r="B166">
-        <v>64.28096782915938</v>
-      </c>
-      <c r="C166">
-        <v>51.877841712857247</v>
-      </c>
-      <c r="D166">
-        <v>4.8422037206810273</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4">
-      <c r="A167">
-        <v>4751.8389999999999</v>
-      </c>
-      <c r="B167">
-        <v>63.791259434470064</v>
-      </c>
-      <c r="C167">
-        <v>52.412991855132738</v>
-      </c>
-      <c r="D167">
-        <v>4.8529897763491503</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
-      <c r="A168">
-        <v>4780.9880000000003</v>
-      </c>
-      <c r="B168">
-        <v>64.462259379255329</v>
-      </c>
-      <c r="C168">
-        <v>53.49524479569353</v>
-      </c>
-      <c r="D168">
-        <v>4.8483401082320974</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
-      <c r="A169">
-        <v>4810.0340000000006</v>
-      </c>
-      <c r="B169">
-        <v>64.692534598189624</v>
-      </c>
-      <c r="C169">
-        <v>53.935675301473964</v>
-      </c>
-      <c r="D169">
-        <v>4.85712116104275</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4">
-      <c r="A170">
-        <v>4838.8969999999999</v>
-      </c>
-      <c r="B170">
-        <v>64.058645323999656</v>
-      </c>
-      <c r="C170">
-        <v>54.189429620843292</v>
-      </c>
-      <c r="D170">
-        <v>4.8519038693838192</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
-      <c r="A171">
-        <v>4867.982</v>
-      </c>
-      <c r="B171">
-        <v>64.151772191433977</v>
-      </c>
-      <c r="C171">
-        <v>54.850368540282581</v>
-      </c>
-      <c r="D171">
-        <v>4.8545338671390006</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4">
-      <c r="A172">
-        <v>4897.0550000000003</v>
-      </c>
-      <c r="B172">
-        <v>64.66540960298434</v>
-      </c>
-      <c r="C172">
-        <v>55.465159142833365</v>
-      </c>
-      <c r="D172">
-        <v>4.8537975048463755</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4">
-      <c r="A173">
-        <v>4925.83</v>
-      </c>
-      <c r="B173">
-        <v>64.255996911994103</v>
-      </c>
-      <c r="C173">
-        <v>56.377323598066518</v>
-      </c>
-      <c r="D173">
-        <v>4.8481841559576919</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
-      <c r="A174">
-        <v>4954.8460000000005</v>
-      </c>
-      <c r="B174">
-        <v>64.572623655856205</v>
-      </c>
-      <c r="C174">
-        <v>54.565007221268246</v>
-      </c>
-      <c r="D174">
-        <v>4.846796318406736</v>
-      </c>
-    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>